<commit_message>
Changed fNearDistance for VampireLord and Werewolf to 15.0
Updated spreadsheet with removed addresses.
</commit_message>
<xml_diff>
--- a/assets/Misc/improvedcamera-addresses.xlsx
+++ b/assets/Misc/improvedcamera-addresses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="375">
   <si>
     <t xml:space="preserve">Signature match, may also be using offsets +/-.</t>
   </si>
@@ -1254,7 +1254,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1340,10 +1340,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1483,7 +1479,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.91"/>
   </cols>
@@ -1538,7 +1534,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="22.82"/>
@@ -1939,119 +1935,113 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="n">
+      <c r="A11" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="M11" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="n">
+      <c r="A12" s="15" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12" t="s">
+      <c r="F12" s="16"/>
+      <c r="G12" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="M12" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="n">
+      <c r="A13" s="15" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="M13" s="12" t="s">
+      <c r="M13" s="16" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2130,80 +2120,76 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="n">
+      <c r="A16" s="15" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12" t="s">
+      <c r="F16" s="16"/>
+      <c r="G16" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="M16" s="12" t="s">
+      <c r="M16" s="16" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="n">
+      <c r="A17" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12" t="s">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="M17" s="12" t="s">
+      <c r="M17" s="16" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3193,7 +3179,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="15" t="n">
         <v>43</v>
       </c>
@@ -3361,7 +3347,7 @@
       <c r="C48" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="D48" s="23" t="s">
+      <c r="D48" s="22" t="s">
         <v>255</v>
       </c>
       <c r="E48" s="12" t="s">
@@ -3391,80 +3377,76 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="11" t="n">
+      <c r="A49" s="15" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="C49" s="13" t="s">
+      <c r="B49" s="16"/>
+      <c r="C49" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12" t="s">
+      <c r="F49" s="16"/>
+      <c r="G49" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="H49" s="12" t="s">
+      <c r="H49" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="I49" s="12" t="s">
+      <c r="I49" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="J49" s="12" t="s">
+      <c r="J49" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="K49" s="12" t="s">
+      <c r="K49" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="L49" s="12" t="s">
+      <c r="L49" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="M49" s="12" t="s">
+      <c r="M49" s="16" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="11" t="n">
+      <c r="A50" s="15" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="C50" s="13" t="s">
+      <c r="B50" s="16"/>
+      <c r="C50" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12" t="s">
+      <c r="F50" s="16"/>
+      <c r="G50" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H50" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="I50" s="12" t="s">
+      <c r="I50" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="J50" s="12" t="s">
+      <c r="J50" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="K50" s="12" t="s">
+      <c r="K50" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="L50" s="12" t="s">
+      <c r="L50" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="M50" s="12" t="s">
+      <c r="M50" s="16" t="s">
         <v>266</v>
       </c>
     </row>
@@ -3508,164 +3490,162 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="11" t="n">
+      <c r="A52" s="15" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="16"/>
+      <c r="C52" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="I52" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="J52" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="K52" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="L52" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="M52" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="23" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="I52" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="J52" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="K52" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="L52" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="M52" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="24" t="n">
-        <v>52</v>
-      </c>
-      <c r="B53" s="25" t="s">
+      <c r="C53" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="F53" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="G53" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="H53" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="I53" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="J53" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="K53" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="L53" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="M53" s="24" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="23" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C53" s="26" t="s">
-        <v>279</v>
-      </c>
-      <c r="D53" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="E53" s="25" t="s">
-        <v>281</v>
-      </c>
-      <c r="F53" s="25" t="s">
+      <c r="C54" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="E54" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="F54" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="G53" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="H53" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="I53" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="J53" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="K53" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="L53" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="M53" s="25" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="24" t="n">
-        <v>53</v>
-      </c>
-      <c r="B54" s="25" t="s">
+      <c r="G54" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="H54" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="I54" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="J54" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="K54" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="L54" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="M54" s="24" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="23" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C54" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="D54" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="E54" s="25" t="s">
-        <v>287</v>
-      </c>
-      <c r="F54" s="25" t="s">
+      <c r="C55" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="F55" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="G54" s="25" t="s">
-        <v>288</v>
-      </c>
-      <c r="H54" s="25" t="s">
-        <v>288</v>
-      </c>
-      <c r="I54" s="25" t="s">
-        <v>288</v>
-      </c>
-      <c r="J54" s="25" t="s">
-        <v>288</v>
-      </c>
-      <c r="K54" s="25" t="s">
-        <v>289</v>
-      </c>
-      <c r="L54" s="25" t="s">
-        <v>289</v>
-      </c>
-      <c r="M54" s="25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="24" t="n">
-        <v>54</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="E55" s="25" t="s">
-        <v>292</v>
-      </c>
-      <c r="F55" s="25" t="s">
-        <v>282</v>
-      </c>
-      <c r="G55" s="25" t="s">
+      <c r="G55" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="H55" s="25" t="s">
+      <c r="H55" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="I55" s="25" t="s">
+      <c r="I55" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="J55" s="25" t="s">
+      <c r="J55" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="K55" s="25" t="s">
+      <c r="K55" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="L55" s="25" t="s">
+      <c r="L55" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="M55" s="25" t="s">
+      <c r="M55" s="24" t="s">
         <v>294</v>
       </c>
     </row>
@@ -3751,243 +3731,243 @@
       <c r="A58" s="15" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="27"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="17" t="s">
         <v>306</v>
       </c>
       <c r="D58" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="E58" s="28" t="s">
+      <c r="E58" s="27" t="s">
         <v>308</v>
       </c>
-      <c r="F58" s="27" t="s">
+      <c r="F58" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="G58" s="27" t="s">
+      <c r="G58" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="H58" s="27" t="s">
+      <c r="H58" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="I58" s="27" t="s">
+      <c r="I58" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="J58" s="27" t="s">
+      <c r="J58" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="K58" s="27" t="s">
+      <c r="K58" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="L58" s="27" t="s">
+      <c r="L58" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="M58" s="27" t="s">
+      <c r="M58" s="26" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="24" t="n">
+      <c r="A59" s="23" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="25" t="s">
+      <c r="B59" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C59" s="26" t="s">
+      <c r="C59" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="D59" s="26" t="s">
+      <c r="D59" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="E59" s="25" t="s">
+      <c r="E59" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="F59" s="25" t="s">
+      <c r="F59" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="G59" s="25" t="s">
+      <c r="G59" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="H59" s="25" t="s">
+      <c r="H59" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="I59" s="25" t="s">
+      <c r="I59" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="J59" s="25" t="s">
+      <c r="J59" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="K59" s="25" t="s">
+      <c r="K59" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="L59" s="25" t="s">
+      <c r="L59" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="M59" s="25" t="s">
+      <c r="M59" s="24" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="24" t="n">
+      <c r="A60" s="23" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="25" t="s">
+      <c r="B60" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="D60" s="29" t="s">
+      <c r="D60" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="E60" s="30" t="s">
+      <c r="E60" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="F60" s="25" t="s">
+      <c r="F60" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="G60" s="25" t="s">
+      <c r="G60" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="H60" s="25" t="s">
+      <c r="H60" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="I60" s="25" t="s">
+      <c r="I60" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="J60" s="25" t="s">
+      <c r="J60" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="K60" s="30" t="s">
+      <c r="K60" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="L60" s="30" t="s">
+      <c r="L60" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="M60" s="30" t="s">
+      <c r="M60" s="29" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24" t="n">
+      <c r="A61" s="23" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="D61" s="26" t="s">
+      <c r="D61" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="E61" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="F61" s="25" t="s">
+      <c r="F61" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="G61" s="25" t="s">
+      <c r="G61" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="H61" s="25" t="s">
+      <c r="H61" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="I61" s="25" t="s">
+      <c r="I61" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="J61" s="25" t="s">
+      <c r="J61" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="K61" s="25" t="s">
+      <c r="K61" s="24" t="s">
         <v>326</v>
       </c>
-      <c r="L61" s="25" t="s">
+      <c r="L61" s="24" t="s">
         <v>326</v>
       </c>
-      <c r="M61" s="25" t="s">
+      <c r="M61" s="24" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="24" t="n">
+      <c r="A62" s="23" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="25" t="s">
+      <c r="B62" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C62" s="26" t="s">
+      <c r="C62" s="25" t="s">
         <v>327</v>
       </c>
-      <c r="D62" s="26" t="s">
+      <c r="D62" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="E62" s="30" t="s">
+      <c r="E62" s="29" t="s">
         <v>329</v>
       </c>
-      <c r="F62" s="25" t="s">
+      <c r="F62" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="G62" s="25" t="s">
+      <c r="G62" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="H62" s="25" t="s">
+      <c r="H62" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="I62" s="25" t="s">
+      <c r="I62" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="J62" s="25" t="s">
+      <c r="J62" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="K62" s="25" t="s">
+      <c r="K62" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="L62" s="25" t="s">
+      <c r="L62" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="M62" s="25" t="s">
+      <c r="M62" s="24" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="24" t="n">
+      <c r="A63" s="23" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C63" s="26" t="s">
+      <c r="C63" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="D63" s="26" t="s">
+      <c r="D63" s="25" t="s">
         <v>333</v>
       </c>
-      <c r="E63" s="30" t="s">
+      <c r="E63" s="29" t="s">
         <v>334</v>
       </c>
-      <c r="F63" s="25" t="s">
+      <c r="F63" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="G63" s="25" t="s">
+      <c r="G63" s="24" t="s">
         <v>335</v>
       </c>
-      <c r="H63" s="25" t="s">
+      <c r="H63" s="24" t="s">
         <v>335</v>
       </c>
-      <c r="I63" s="25" t="s">
+      <c r="I63" s="24" t="s">
         <v>335</v>
       </c>
-      <c r="J63" s="25" t="s">
+      <c r="J63" s="24" t="s">
         <v>335</v>
       </c>
-      <c r="K63" s="25" t="s">
+      <c r="K63" s="24" t="s">
         <v>336</v>
       </c>
-      <c r="L63" s="25" t="s">
+      <c r="L63" s="24" t="s">
         <v>336</v>
       </c>
-      <c r="M63" s="25" t="s">
+      <c r="M63" s="24" t="s">
         <v>336</v>
       </c>
     </row>
@@ -4031,207 +4011,207 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="24" t="n">
+      <c r="A65" s="23" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B65" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="C65" s="25" t="s">
         <v>342</v>
       </c>
-      <c r="D65" s="26" t="s">
+      <c r="D65" s="25" t="s">
         <v>343</v>
       </c>
-      <c r="E65" s="25" t="s">
+      <c r="E65" s="24" t="s">
         <v>344</v>
       </c>
-      <c r="F65" s="25" t="s">
+      <c r="F65" s="24" t="s">
         <v>345</v>
       </c>
-      <c r="G65" s="25" t="s">
+      <c r="G65" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="H65" s="25" t="s">
+      <c r="H65" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="I65" s="25" t="s">
+      <c r="I65" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="J65" s="25" t="s">
+      <c r="J65" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="K65" s="25" t="s">
+      <c r="K65" s="24" t="s">
         <v>347</v>
       </c>
-      <c r="L65" s="25" t="s">
+      <c r="L65" s="24" t="s">
         <v>347</v>
       </c>
-      <c r="M65" s="25" t="s">
+      <c r="M65" s="24" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="24" t="n">
+      <c r="A66" s="23" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="25" t="s">
+      <c r="B66" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="25" t="s">
         <v>348</v>
       </c>
-      <c r="D66" s="26" t="s">
+      <c r="D66" s="25" t="s">
         <v>349</v>
       </c>
-      <c r="E66" s="25" t="s">
+      <c r="E66" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="F66" s="25" t="s">
+      <c r="F66" s="24" t="s">
         <v>303</v>
       </c>
-      <c r="G66" s="25" t="s">
+      <c r="G66" s="24" t="s">
         <v>351</v>
       </c>
-      <c r="H66" s="25" t="s">
+      <c r="H66" s="24" t="s">
         <v>351</v>
       </c>
-      <c r="I66" s="25" t="s">
+      <c r="I66" s="24" t="s">
         <v>351</v>
       </c>
-      <c r="J66" s="25" t="s">
+      <c r="J66" s="24" t="s">
         <v>351</v>
       </c>
-      <c r="K66" s="25" t="s">
+      <c r="K66" s="24" t="s">
         <v>352</v>
       </c>
-      <c r="L66" s="25" t="s">
+      <c r="L66" s="24" t="s">
         <v>352</v>
       </c>
-      <c r="M66" s="25" t="s">
+      <c r="M66" s="24" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="24" t="n">
+      <c r="A67" s="23" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="25" t="s">
+      <c r="B67" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="25" t="s">
         <v>353</v>
       </c>
-      <c r="D67" s="26" t="s">
+      <c r="D67" s="25" t="s">
         <v>354</v>
       </c>
-      <c r="E67" s="25" t="s">
+      <c r="E67" s="24" t="s">
         <v>355</v>
       </c>
-      <c r="F67" s="25" t="s">
+      <c r="F67" s="24" t="s">
         <v>303</v>
       </c>
-      <c r="G67" s="25" t="s">
+      <c r="G67" s="24" t="s">
         <v>356</v>
       </c>
-      <c r="H67" s="25" t="s">
+      <c r="H67" s="24" t="s">
         <v>356</v>
       </c>
-      <c r="I67" s="25" t="s">
+      <c r="I67" s="24" t="s">
         <v>356</v>
       </c>
-      <c r="J67" s="25" t="s">
+      <c r="J67" s="24" t="s">
         <v>356</v>
       </c>
-      <c r="K67" s="25" t="s">
+      <c r="K67" s="24" t="s">
         <v>357</v>
       </c>
-      <c r="L67" s="25" t="s">
+      <c r="L67" s="24" t="s">
         <v>357</v>
       </c>
-      <c r="M67" s="25" t="s">
+      <c r="M67" s="24" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="24" t="n">
+      <c r="A68" s="23" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="B68" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C68" s="26" t="s">
+      <c r="C68" s="25" t="s">
         <v>358</v>
       </c>
-      <c r="D68" s="26" t="s">
+      <c r="D68" s="25" t="s">
         <v>359</v>
       </c>
-      <c r="E68" s="25" t="s">
+      <c r="E68" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="F68" s="25" t="s">
+      <c r="F68" s="24" t="s">
         <v>303</v>
       </c>
-      <c r="G68" s="25" t="s">
+      <c r="G68" s="24" t="s">
         <v>361</v>
       </c>
-      <c r="H68" s="25" t="s">
+      <c r="H68" s="24" t="s">
         <v>361</v>
       </c>
-      <c r="I68" s="25" t="s">
+      <c r="I68" s="24" t="s">
         <v>361</v>
       </c>
-      <c r="J68" s="25" t="s">
+      <c r="J68" s="24" t="s">
         <v>361</v>
       </c>
-      <c r="K68" s="25" t="s">
+      <c r="K68" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="L68" s="25" t="s">
+      <c r="L68" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="M68" s="25" t="s">
+      <c r="M68" s="24" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="24" t="n">
+      <c r="A69" s="23" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="25" t="s">
+      <c r="B69" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C69" s="26" t="s">
+      <c r="C69" s="25" t="s">
         <v>363</v>
       </c>
-      <c r="D69" s="26" t="s">
+      <c r="D69" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="E69" s="30" t="s">
+      <c r="E69" s="29" t="s">
         <v>365</v>
       </c>
-      <c r="F69" s="25" t="s">
+      <c r="F69" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="G69" s="25" t="s">
+      <c r="G69" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="H69" s="25" t="s">
+      <c r="H69" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="I69" s="25" t="s">
+      <c r="I69" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="J69" s="25" t="s">
+      <c r="J69" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="K69" s="25" t="s">
+      <c r="K69" s="24" t="s">
         <v>367</v>
       </c>
-      <c r="L69" s="25" t="s">
+      <c r="L69" s="24" t="s">
         <v>367</v>
       </c>
-      <c r="M69" s="25" t="s">
+      <c r="M69" s="24" t="s">
         <v>367</v>
       </c>
     </row>
@@ -4543,7 +4523,7 @@
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D109" s="2"/>
       <c r="E109" s="7"/>
-      <c r="J109" s="31"/>
+      <c r="J109" s="30"/>
       <c r="M109" s="7"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4661,7 +4641,7 @@
       <c r="M134" s="7"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D135" s="32"/>
+      <c r="D135" s="31"/>
       <c r="E135" s="7"/>
       <c r="M135" s="7"/>
     </row>
@@ -4684,7 +4664,7 @@
       <c r="M139" s="7"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D140" s="32"/>
+      <c r="D140" s="31"/>
       <c r="M140" s="7"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4697,7 +4677,7 @@
       <c r="M142" s="7"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D143" s="32"/>
+      <c r="D143" s="31"/>
       <c r="E143" s="7"/>
       <c r="M143" s="7"/>
     </row>
@@ -4821,7 +4801,7 @@
       <c r="M169" s="7"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D170" s="32"/>
+      <c r="D170" s="31"/>
       <c r="M170" s="7"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5028,31 +5008,31 @@
       <c r="M214" s="7"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D215" s="32"/>
+      <c r="D215" s="31"/>
       <c r="E215" s="7"/>
       <c r="M215" s="7"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D216" s="32"/>
+      <c r="D216" s="31"/>
       <c r="E216" s="7"/>
       <c r="M216" s="7"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D217" s="32"/>
+      <c r="D217" s="31"/>
       <c r="M217" s="7"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D218" s="32"/>
+      <c r="D218" s="31"/>
       <c r="E218" s="7"/>
       <c r="M218" s="7"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D219" s="32"/>
+      <c r="D219" s="31"/>
       <c r="E219" s="7"/>
       <c r="M219" s="7"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D220" s="32"/>
+      <c r="D220" s="31"/>
       <c r="E220" s="7"/>
       <c r="M220" s="7"/>
     </row>
@@ -5062,7 +5042,7 @@
       <c r="M221" s="7"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D222" s="32"/>
+      <c r="D222" s="31"/>
       <c r="M222" s="7"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5071,7 +5051,7 @@
       <c r="M223" s="7"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D224" s="32"/>
+      <c r="D224" s="31"/>
       <c r="M224" s="7"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5080,7 +5060,7 @@
       <c r="M225" s="7"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D226" s="32"/>
+      <c r="D226" s="31"/>
       <c r="M226" s="7"/>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5094,19 +5074,19 @@
       <c r="M228" s="7"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D229" s="32"/>
+      <c r="D229" s="31"/>
       <c r="M229" s="7"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D230" s="32"/>
+      <c r="D230" s="31"/>
       <c r="M230" s="7"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D231" s="32"/>
+      <c r="D231" s="31"/>
       <c r="M231" s="7"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D232" s="32"/>
+      <c r="D232" s="31"/>
       <c r="M232" s="7"/>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5119,28 +5099,28 @@
       <c r="M234" s="7"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D235" s="32"/>
+      <c r="D235" s="31"/>
       <c r="M235" s="7"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D236" s="32"/>
+      <c r="D236" s="31"/>
       <c r="M236" s="7"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D237" s="32"/>
+      <c r="D237" s="31"/>
       <c r="M237" s="7"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D238" s="32"/>
+      <c r="D238" s="31"/>
       <c r="M238" s="7"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D239" s="32"/>
+      <c r="D239" s="31"/>
       <c r="E239" s="7"/>
       <c r="M239" s="7"/>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D240" s="32"/>
+      <c r="D240" s="31"/>
       <c r="E240" s="7"/>
       <c r="M240" s="7"/>
     </row>
@@ -5178,23 +5158,23 @@
       <c r="M247" s="7"/>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D248" s="32"/>
+      <c r="D248" s="31"/>
       <c r="M248" s="7"/>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D249" s="32"/>
+      <c r="D249" s="31"/>
       <c r="M249" s="7"/>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D250" s="32"/>
+      <c r="D250" s="31"/>
       <c r="M250" s="7"/>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D251" s="32"/>
+      <c r="D251" s="31"/>
       <c r="M251" s="7"/>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D252" s="32"/>
+      <c r="D252" s="31"/>
       <c r="M252" s="7"/>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5202,15 +5182,15 @@
       <c r="M253" s="7"/>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D254" s="32"/>
+      <c r="D254" s="31"/>
       <c r="M254" s="7"/>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D255" s="32"/>
+      <c r="D255" s="31"/>
       <c r="M255" s="7"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D256" s="32"/>
+      <c r="D256" s="31"/>
       <c r="E256" s="7"/>
       <c r="M256" s="7"/>
     </row>
@@ -5233,11 +5213,11 @@
       <c r="M260" s="7"/>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D261" s="32"/>
+      <c r="D261" s="31"/>
       <c r="M261" s="7"/>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D262" s="32"/>
+      <c r="D262" s="31"/>
       <c r="E262" s="7"/>
       <c r="M262" s="7"/>
     </row>
@@ -5343,7 +5323,7 @@
       <c r="M284" s="7"/>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D285" s="32"/>
+      <c r="D285" s="31"/>
       <c r="E285" s="7"/>
       <c r="M285" s="7"/>
     </row>
@@ -5371,7 +5351,7 @@
       <c r="M290" s="7"/>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D291" s="32"/>
+      <c r="D291" s="31"/>
       <c r="E291" s="7"/>
       <c r="M291" s="7"/>
     </row>

</xml_diff>